<commit_message>
Creacion de evidencia, plan de prueba, y cambios en strings de los it del codigo
</commit_message>
<xml_diff>
--- a/Plan de prueba.xlsx
+++ b/Plan de prueba.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farid\OneDrive\Desktop\EntregaFinal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D012426-DAE2-4C92-89B4-C211107AC01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,167 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+  <si>
+    <t>Realizado por: Farid Ale Ali</t>
+  </si>
+  <si>
+    <t>Módulo/Pantalla/Sprint: Compra de usuarios en Sauce Demo</t>
+  </si>
+  <si>
+    <t>Respaldado por: Cypress</t>
+  </si>
+  <si>
+    <t>Iteración I</t>
+  </si>
+  <si>
+    <t>Iteración II</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>JIRA ID</t>
+  </si>
+  <si>
+    <t>Caso gral</t>
+  </si>
+  <si>
+    <t>Descripción del caso.</t>
+  </si>
+  <si>
+    <t>Pasos a seguir</t>
+  </si>
+  <si>
+    <t>Resultado Esperado</t>
+  </si>
+  <si>
+    <t>Ejecutado
+S/N</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Imagen</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Tkt</t>
+  </si>
+  <si>
+    <t>Ticket JIRA ID</t>
+  </si>
+  <si>
+    <t>SD-101</t>
+  </si>
+  <si>
+    <t>1. Iniciar sesión con el usuario standard_user.
+2. Seleccionar los productos disponibles.
+3. Acceder al carrito de compras.
+4. Proceder al checkout.
+5. Completar la información de envío.
+6. Finalizar la compra.
+7. Cerrar sesión.</t>
+  </si>
+  <si>
+    <t>El usuario debería poder completar el proceso de compra sin errores y ver la pantalla de confirmación de compra.</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>La prueba pasa correctamente, observar:
+1. Uno de los productos tiene un nombre incorrecto</t>
+  </si>
+  <si>
+    <t>SD-102</t>
+  </si>
+  <si>
+    <t>1. Iniciar sesión con el usuario problem_user.
+2. Seleccionar los productos disponibles.
+3. Acceder al carrito de compras.
+4. Proceder al checkout.
+5. Completar la información de envío.
+6. Finalizar la compra.
+7. Cerrar sesión.</t>
+  </si>
+  <si>
+    <t>La prueba no pasa correctamente: 
+1. De los 6 productos, solo 3 funcionan al agregar al carrito y los otros 3 no funcionan.
+3. Uno de los productos tiene un nombre incorrecto
+2. El input de "Last Name" es erroneo, tiene un error de funcionalidad</t>
+  </si>
+  <si>
+    <t>SD-104</t>
+  </si>
+  <si>
+    <t>El bug anterior persiste</t>
+  </si>
+  <si>
+    <t>Verificar que un usuario con un pueda realizar una compra con éxito.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se inicia sesión con un usuario </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(standard_user)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>, se seleccionan productos y se realiza la compra.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se inicia sesión con un usuario </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(problem_user)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>, se seleccionan productos y se realiza la compra.</t>
+    </r>
+  </si>
+  <si>
+    <t>Observaciones: Pruebas automáticas de flujo de compra con diferentes usuarios.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +192,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666666"/>
+        <bgColor rgb="FF666666"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -45,12 +256,198 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +727,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="50.7109375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12" style="11" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="19"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="22"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="K5:N5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>